<commit_message>
Updated test matrix w/ crop size
</commit_message>
<xml_diff>
--- a/TestMatrix.xlsx
+++ b/TestMatrix.xlsx
@@ -527,8 +527,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9:M12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -659,7 +659,7 @@
         <v>10</v>
       </c>
       <c r="G5">
-        <v>120</v>
+        <v>224</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -682,7 +682,7 @@
         <v>10</v>
       </c>
       <c r="G6">
-        <v>120</v>
+        <v>224</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3"/>
@@ -805,7 +805,7 @@
         <v>10</v>
       </c>
       <c r="G11">
-        <v>120</v>
+        <v>224</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
@@ -828,7 +828,7 @@
         <v>10</v>
       </c>
       <c r="G12">
-        <v>120</v>
+        <v>224</v>
       </c>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>

</xml_diff>

<commit_message>
Updated test matrix w/ fixed numbers
</commit_message>
<xml_diff>
--- a/TestMatrix.xlsx
+++ b/TestMatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="80" windowWidth="14400" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="65">
   <si>
     <t>Assignee</t>
   </si>
@@ -76,6 +76,144 @@
   </si>
   <si>
     <t>30K Accuracy (New)</t>
+  </si>
+  <si>
+    <t>Fixed Labels</t>
+  </si>
+  <si>
+    <t>Wrong Labels</t>
+  </si>
+  <si>
+    <t>'Acura'</t>
+  </si>
+  <si>
+    <t>'Aston'</t>
+  </si>
+  <si>
+    <t>'Audi'</t>
+  </si>
+  <si>
+    <t>'BMW'</t>
+  </si>
+  <si>
+    <t>'Bentley'</t>
+  </si>
+  <si>
+    <t>'Bugatti'</t>
+  </si>
+  <si>
+    <t>'Buick'</t>
+  </si>
+  <si>
+    <t>'Cadillac'</t>
+  </si>
+  <si>
+    <t>'Chevrolet'</t>
+  </si>
+  <si>
+    <t>'Chrysler'</t>
+  </si>
+  <si>
+    <t>'Daewoo'</t>
+  </si>
+  <si>
+    <t>'Dodge'</t>
+  </si>
+  <si>
+    <t>'FIAT'</t>
+  </si>
+  <si>
+    <t>'Ferrari'</t>
+  </si>
+  <si>
+    <t>'Ford'</t>
+  </si>
+  <si>
+    <t>'GMC'</t>
+  </si>
+  <si>
+    <t>'HUMMER'</t>
+  </si>
+  <si>
+    <t>'Honda'</t>
+  </si>
+  <si>
+    <t>'Hyundai'</t>
+  </si>
+  <si>
+    <t>'Infiniti'</t>
+  </si>
+  <si>
+    <t>'Jaguar'</t>
+  </si>
+  <si>
+    <t>'Jeep'</t>
+  </si>
+  <si>
+    <t>'Lamborghini'</t>
+  </si>
+  <si>
+    <t>'Land'</t>
+  </si>
+  <si>
+    <t>'Lincoln'</t>
+  </si>
+  <si>
+    <t>'MINI'</t>
+  </si>
+  <si>
+    <t>'Mazda'</t>
+  </si>
+  <si>
+    <t>'McLaren'</t>
+  </si>
+  <si>
+    <t>'Mercedes-Benz'</t>
+  </si>
+  <si>
+    <t>'Mitsubishi'</t>
+  </si>
+  <si>
+    <t>'Nissan'</t>
+  </si>
+  <si>
+    <t>'Porsche'</t>
+  </si>
+  <si>
+    <t>'Ram'</t>
+  </si>
+  <si>
+    <t>'Rolls-Royce'</t>
+  </si>
+  <si>
+    <t>'Suzuki'</t>
+  </si>
+  <si>
+    <t>'Tesla'</t>
+  </si>
+  <si>
+    <t>'Toyota'</t>
+  </si>
+  <si>
+    <t>'Volkswagen'</t>
+  </si>
+  <si>
+    <t>'Volvo'</t>
+  </si>
+  <si>
+    <t>'smart'</t>
+  </si>
+  <si>
+    <t>Flickr/128/0</t>
+  </si>
+  <si>
+    <t>Flickr/128/.5</t>
+  </si>
+  <si>
+    <t>Flickr/256/0</t>
+  </si>
+  <si>
+    <t>Flickr/256/.5</t>
   </si>
 </sst>
 </file>
@@ -126,12 +264,48 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFBD3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -143,7 +317,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -159,12 +333,17 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -177,11 +356,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -189,6 +371,7 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -196,6 +379,7 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -525,14 +709,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M14"/>
+  <dimension ref="A1:Q58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H2" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+    <sheetView tabSelected="1" topLeftCell="B15" workbookViewId="0">
+      <selection activeCell="Q15" sqref="Q15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="17.6640625" customWidth="1"/>
     <col min="6" max="6" width="8.5" customWidth="1"/>
     <col min="7" max="7" width="8.6640625" customWidth="1"/>
     <col min="8" max="8" width="12" customWidth="1"/>
@@ -543,16 +728,28 @@
     <col min="13" max="13" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13">
-      <c r="A1" s="8" t="s">
+    <row r="1" spans="1:17">
+      <c r="A1" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="8"/>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-    </row>
-    <row r="2" spans="1:13">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="J1" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
+      <c r="M1" s="4"/>
+      <c r="N1" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="O1" s="4"/>
+      <c r="P1" s="4"/>
+      <c r="Q1" s="4"/>
+    </row>
+    <row r="2" spans="1:17">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -592,15 +789,27 @@
       <c r="M2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:13">
-      <c r="A3" s="5" t="s">
+      <c r="N2" t="s">
+        <v>15</v>
+      </c>
+      <c r="O2" t="s">
+        <v>16</v>
+      </c>
+      <c r="P2" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17">
+      <c r="A3" s="6" t="s">
         <v>6</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="7" t="s">
         <v>8</v>
       </c>
       <c r="D3">
@@ -619,13 +828,17 @@
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
       <c r="M3" s="3"/>
-    </row>
-    <row r="4" spans="1:13">
-      <c r="A4" s="5"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+    </row>
+    <row r="4" spans="1:17">
+      <c r="A4" s="6"/>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="6"/>
+      <c r="C4" s="7"/>
       <c r="D4">
         <v>256</v>
       </c>
@@ -642,13 +855,17 @@
       <c r="K4" s="3"/>
       <c r="L4" s="3"/>
       <c r="M4" s="3"/>
-    </row>
-    <row r="5" spans="1:13">
-      <c r="A5" s="5"/>
+      <c r="N4" s="3"/>
+      <c r="O4" s="3"/>
+      <c r="P4" s="3"/>
+      <c r="Q4" s="3"/>
+    </row>
+    <row r="5" spans="1:17">
+      <c r="A5" s="6"/>
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="6"/>
+      <c r="C5" s="7"/>
       <c r="D5">
         <v>128</v>
       </c>
@@ -665,13 +882,17 @@
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="M5" s="3"/>
-    </row>
-    <row r="6" spans="1:13">
-      <c r="A6" s="5"/>
+      <c r="N5" s="3"/>
+      <c r="O5" s="3"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="3"/>
+    </row>
+    <row r="6" spans="1:17">
+      <c r="A6" s="6"/>
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" s="6"/>
+      <c r="C6" s="7"/>
       <c r="D6">
         <v>128</v>
       </c>
@@ -688,37 +909,49 @@
       <c r="K6" s="3"/>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
-    </row>
-    <row r="7" spans="1:13">
-      <c r="A7" s="5"/>
+      <c r="N6" s="3"/>
+      <c r="O6" s="3"/>
+      <c r="P6" s="3"/>
+      <c r="Q6" s="3"/>
+    </row>
+    <row r="7" spans="1:17">
+      <c r="A7" s="6"/>
       <c r="B7">
         <v>5</v>
       </c>
-      <c r="C7" s="6"/>
+      <c r="C7" s="7"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
-    </row>
-    <row r="8" spans="1:13">
-      <c r="A8" s="5"/>
+      <c r="N7" s="3"/>
+      <c r="O7" s="3"/>
+      <c r="P7" s="3"/>
+      <c r="Q7" s="3"/>
+    </row>
+    <row r="8" spans="1:17">
+      <c r="A8" s="6"/>
       <c r="B8">
         <v>6</v>
       </c>
-      <c r="C8" s="6"/>
+      <c r="C8" s="7"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
       <c r="M8" s="3"/>
-    </row>
-    <row r="9" spans="1:13">
-      <c r="A9" s="4" t="s">
+      <c r="N8" s="3"/>
+      <c r="O8" s="3"/>
+      <c r="P8" s="3"/>
+      <c r="Q8" s="3"/>
+    </row>
+    <row r="9" spans="1:17">
+      <c r="A9" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="7" t="s">
+      <c r="C9" s="8" t="s">
         <v>12</v>
       </c>
       <c r="D9">
@@ -751,13 +984,17 @@
       <c r="M9" s="3">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="10" spans="1:13">
-      <c r="A10" s="4"/>
+      <c r="N9" s="3"/>
+      <c r="O9" s="3"/>
+      <c r="P9" s="3"/>
+      <c r="Q9" s="3"/>
+    </row>
+    <row r="10" spans="1:17">
+      <c r="A10" s="5"/>
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" s="7"/>
+      <c r="C10" s="8"/>
       <c r="D10">
         <v>256</v>
       </c>
@@ -788,13 +1025,17 @@
       <c r="M10" s="3">
         <v>0.36</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
-      <c r="A11" s="4"/>
+      <c r="N10" s="3"/>
+      <c r="O10" s="3"/>
+      <c r="P10" s="3"/>
+      <c r="Q10" s="3"/>
+    </row>
+    <row r="11" spans="1:17">
+      <c r="A11" s="5"/>
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" s="7"/>
+      <c r="C11" s="8"/>
       <c r="D11">
         <v>128</v>
       </c>
@@ -819,13 +1060,17 @@
       <c r="M11" s="3">
         <v>0.32500000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:13">
-      <c r="A12" s="4"/>
+      <c r="N11" s="3"/>
+      <c r="O11" s="3"/>
+      <c r="P11" s="3"/>
+      <c r="Q11" s="3"/>
+    </row>
+    <row r="12" spans="1:17">
+      <c r="A12" s="5"/>
       <c r="B12">
         <v>4</v>
       </c>
-      <c r="C12" s="7"/>
+      <c r="C12" s="8"/>
       <c r="D12">
         <v>128</v>
       </c>
@@ -850,23 +1095,371 @@
       <c r="M12" s="3">
         <v>0.34</v>
       </c>
-    </row>
-    <row r="13" spans="1:13">
-      <c r="A13" s="4"/>
+      <c r="N12" s="3">
+        <v>0.79207661025800002</v>
+      </c>
+      <c r="O12" s="3">
+        <v>0.34499999999999997</v>
+      </c>
+      <c r="P12" s="3">
+        <v>0.79378197559999997</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>0.35</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17">
+      <c r="A13" s="5"/>
       <c r="B13">
         <v>5</v>
       </c>
-      <c r="C13" s="7"/>
-    </row>
-    <row r="14" spans="1:13">
-      <c r="A14" s="4"/>
+      <c r="C13" s="8"/>
+    </row>
+    <row r="14" spans="1:17">
+      <c r="A14" s="5"/>
       <c r="B14">
         <v>6</v>
       </c>
-      <c r="C14" s="7"/>
+      <c r="C14" s="8"/>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="B18" t="s">
+        <v>61</v>
+      </c>
+      <c r="C18" t="s">
+        <v>62</v>
+      </c>
+      <c r="D18" t="s">
+        <v>63</v>
+      </c>
+      <c r="E18" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>21</v>
+      </c>
+      <c r="B19" s="12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B21" s="13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>24</v>
+      </c>
+      <c r="B22" s="13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>25</v>
+      </c>
+      <c r="B23" s="14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>26</v>
+      </c>
+      <c r="B24" s="12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>27</v>
+      </c>
+      <c r="B25" s="13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>28</v>
+      </c>
+      <c r="B26" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B27" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>30</v>
+      </c>
+      <c r="B28" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>31</v>
+      </c>
+      <c r="B29" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>33</v>
+      </c>
+      <c r="B31" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>34</v>
+      </c>
+      <c r="B32" s="13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2">
+      <c r="A33" t="s">
+        <v>35</v>
+      </c>
+      <c r="B33" s="11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2">
+      <c r="A34" t="s">
+        <v>36</v>
+      </c>
+      <c r="B34" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2">
+      <c r="A35" t="s">
+        <v>37</v>
+      </c>
+      <c r="B35" s="13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2">
+      <c r="A36" t="s">
+        <v>38</v>
+      </c>
+      <c r="B36" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2">
+      <c r="A37" t="s">
+        <v>39</v>
+      </c>
+      <c r="B37" s="13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2">
+      <c r="A38" t="s">
+        <v>40</v>
+      </c>
+      <c r="B38" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2">
+      <c r="A39" t="s">
+        <v>41</v>
+      </c>
+      <c r="B39" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2">
+      <c r="A40" t="s">
+        <v>42</v>
+      </c>
+      <c r="B40" s="13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="41" spans="1:2">
+      <c r="A41" t="s">
+        <v>43</v>
+      </c>
+      <c r="B41" s="13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="42" spans="1:2">
+      <c r="A42" t="s">
+        <v>44</v>
+      </c>
+      <c r="B42" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="43" spans="1:2">
+      <c r="A43" t="s">
+        <v>45</v>
+      </c>
+      <c r="B43" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:2">
+      <c r="A44" t="s">
+        <v>46</v>
+      </c>
+      <c r="B44" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:2">
+      <c r="A45" t="s">
+        <v>47</v>
+      </c>
+      <c r="B45" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:2">
+      <c r="A46" t="s">
+        <v>48</v>
+      </c>
+      <c r="B46" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="47" spans="1:2">
+      <c r="A47" t="s">
+        <v>49</v>
+      </c>
+      <c r="B47" s="11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:2">
+      <c r="A48" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2">
+      <c r="A49" t="s">
+        <v>51</v>
+      </c>
+      <c r="B49" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2">
+      <c r="A50" t="s">
+        <v>52</v>
+      </c>
+      <c r="B50" s="13">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2">
+      <c r="A51" t="s">
+        <v>53</v>
+      </c>
+      <c r="B51" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2">
+      <c r="A52" t="s">
+        <v>54</v>
+      </c>
+      <c r="B52" s="12">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2">
+      <c r="A53" t="s">
+        <v>55</v>
+      </c>
+      <c r="B53" s="11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2">
+      <c r="A54" t="s">
+        <v>56</v>
+      </c>
+      <c r="B54" s="11">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2">
+      <c r="A55" t="s">
+        <v>57</v>
+      </c>
+      <c r="B55" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2">
+      <c r="A56" t="s">
+        <v>58</v>
+      </c>
+      <c r="B56" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2">
+      <c r="A57" t="s">
+        <v>59</v>
+      </c>
+      <c r="B57" s="10">
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2">
+      <c r="A58" t="s">
+        <v>60</v>
+      </c>
+      <c r="B58" s="11">
+        <v>0.4</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="N1:Q1"/>
+    <mergeCell ref="J1:M1"/>
     <mergeCell ref="A9:A14"/>
     <mergeCell ref="A3:A8"/>
     <mergeCell ref="C3:C8"/>

</xml_diff>

<commit_message>
Added an evalutation script for Zahir
</commit_message>
<xml_diff>
--- a/TestMatrix.xlsx
+++ b/TestMatrix.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26819"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15520" tabRatio="500"/>
+    <workbookView xWindow="3260" yWindow="300" windowWidth="25600" windowHeight="15500" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -213,9 +213,6 @@
     <t>Flickr/128/.5 15K</t>
   </si>
   <si>
-    <t>Flickr/128/.5 39K</t>
-  </si>
-  <si>
     <t>Flickr/256/0 15K</t>
   </si>
   <si>
@@ -226,6 +223,9 @@
   </si>
   <si>
     <t>Flickr/256/.5 15K</t>
+  </si>
+  <si>
+    <t>Flickr/128/.5 30K</t>
   </si>
 </sst>
 </file>
@@ -357,6 +357,11 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -371,11 +376,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="17">
@@ -727,7 +727,7 @@
   <dimension ref="A1:Q58"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -748,25 +748,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="J1" s="9" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="J1" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
-      <c r="N1" s="9" t="s">
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
     </row>
     <row r="2" spans="1:17">
       <c r="A2" t="s">
@@ -822,13 +822,13 @@
       </c>
     </row>
     <row r="3" spans="1:17">
-      <c r="A3" s="11" t="s">
+      <c r="A3" s="14" t="s">
         <v>6</v>
       </c>
       <c r="B3">
         <v>1</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="15" t="s">
         <v>8</v>
       </c>
       <c r="D3">
@@ -853,11 +853,11 @@
       <c r="Q3" s="3"/>
     </row>
     <row r="4" spans="1:17">
-      <c r="A4" s="11"/>
+      <c r="A4" s="14"/>
       <c r="B4">
         <v>2</v>
       </c>
-      <c r="C4" s="12"/>
+      <c r="C4" s="15"/>
       <c r="D4">
         <v>256</v>
       </c>
@@ -880,11 +880,11 @@
       <c r="Q4" s="3"/>
     </row>
     <row r="5" spans="1:17">
-      <c r="A5" s="11"/>
+      <c r="A5" s="14"/>
       <c r="B5">
         <v>3</v>
       </c>
-      <c r="C5" s="12"/>
+      <c r="C5" s="15"/>
       <c r="D5">
         <v>128</v>
       </c>
@@ -907,11 +907,11 @@
       <c r="Q5" s="3"/>
     </row>
     <row r="6" spans="1:17">
-      <c r="A6" s="11"/>
+      <c r="A6" s="14"/>
       <c r="B6">
         <v>4</v>
       </c>
-      <c r="C6" s="12"/>
+      <c r="C6" s="15"/>
       <c r="D6">
         <v>128</v>
       </c>
@@ -934,8 +934,8 @@
       <c r="Q6" s="3"/>
     </row>
     <row r="7" spans="1:17">
-      <c r="A7" s="11"/>
-      <c r="C7" s="12"/>
+      <c r="A7" s="14"/>
+      <c r="C7" s="15"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
       <c r="L7" s="3"/>
@@ -946,8 +946,8 @@
       <c r="Q7" s="3"/>
     </row>
     <row r="8" spans="1:17">
-      <c r="A8" s="11"/>
-      <c r="C8" s="12"/>
+      <c r="A8" s="14"/>
+      <c r="C8" s="15"/>
       <c r="J8" s="3"/>
       <c r="K8" s="3"/>
       <c r="L8" s="3"/>
@@ -958,13 +958,13 @@
       <c r="Q8" s="3"/>
     </row>
     <row r="9" spans="1:17">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="13" t="s">
         <v>5</v>
       </c>
       <c r="B9">
         <v>1</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="16" t="s">
         <v>12</v>
       </c>
       <c r="D9">
@@ -1003,11 +1003,11 @@
       <c r="Q9" s="3"/>
     </row>
     <row r="10" spans="1:17">
-      <c r="A10" s="10"/>
+      <c r="A10" s="13"/>
       <c r="B10">
         <v>2</v>
       </c>
-      <c r="C10" s="13"/>
+      <c r="C10" s="16"/>
       <c r="D10">
         <v>256</v>
       </c>
@@ -1044,11 +1044,11 @@
       <c r="Q10" s="3"/>
     </row>
     <row r="11" spans="1:17">
-      <c r="A11" s="10"/>
+      <c r="A11" s="13"/>
       <c r="B11">
         <v>3</v>
       </c>
-      <c r="C11" s="13"/>
+      <c r="C11" s="16"/>
       <c r="D11">
         <v>128</v>
       </c>
@@ -1061,6 +1061,12 @@
       <c r="G11">
         <v>224</v>
       </c>
+      <c r="H11">
+        <v>1E-4</v>
+      </c>
+      <c r="I11">
+        <v>7500</v>
+      </c>
       <c r="J11" s="3">
         <v>0.77908959727100002</v>
       </c>
@@ -1073,17 +1079,25 @@
       <c r="M11" s="3">
         <v>0.32500000000000001</v>
       </c>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3"/>
+      <c r="N11" s="3">
+        <v>0.78105732651199999</v>
+      </c>
+      <c r="O11" s="3">
+        <v>0.34</v>
+      </c>
+      <c r="P11" s="3">
+        <v>0.78223796405599999</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>0.35</v>
+      </c>
     </row>
     <row r="12" spans="1:17">
-      <c r="A12" s="10"/>
+      <c r="A12" s="13"/>
       <c r="B12">
         <v>4</v>
       </c>
-      <c r="C12" s="13"/>
+      <c r="C12" s="16"/>
       <c r="D12">
         <v>128</v>
       </c>
@@ -1096,6 +1110,12 @@
       <c r="G12">
         <v>224</v>
       </c>
+      <c r="H12">
+        <v>1E-4</v>
+      </c>
+      <c r="I12">
+        <v>7500</v>
+      </c>
       <c r="J12" s="3">
         <v>0.78696051423299995</v>
       </c>
@@ -1122,37 +1142,37 @@
       </c>
     </row>
     <row r="13" spans="1:17">
-      <c r="A13" s="10"/>
-      <c r="C13" s="13"/>
+      <c r="A13" s="13"/>
+      <c r="C13" s="16"/>
     </row>
     <row r="14" spans="1:17">
-      <c r="A14" s="10"/>
-      <c r="C14" s="13"/>
+      <c r="A14" s="13"/>
+      <c r="C14" s="16"/>
     </row>
     <row r="18" spans="1:9" ht="40" customHeight="1">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="E18" s="16" t="s">
+      <c r="E18" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="F18" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="G18" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="G18" s="16" t="s">
+      <c r="H18" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I18" s="11" t="s">
         <v>66</v>
-      </c>
-      <c r="H18" s="16" t="s">
-        <v>68</v>
-      </c>
-      <c r="I18" s="16" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:9">
@@ -1239,7 +1259,7 @@
       <c r="B26" s="4">
         <v>0</v>
       </c>
-      <c r="C26" s="14">
+      <c r="C26" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1250,7 +1270,7 @@
       <c r="B27" s="4">
         <v>0</v>
       </c>
-      <c r="C27" s="14">
+      <c r="C27" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1261,7 +1281,7 @@
       <c r="B28" s="4">
         <v>0</v>
       </c>
-      <c r="C28" s="14">
+      <c r="C28" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1272,7 +1292,7 @@
       <c r="B29" s="4">
         <v>0</v>
       </c>
-      <c r="C29" s="14">
+      <c r="C29" s="9">
         <v>0</v>
       </c>
     </row>
@@ -1313,10 +1333,10 @@
       <c r="A33" t="s">
         <v>35</v>
       </c>
-      <c r="B33" s="15">
+      <c r="B33" s="10">
         <v>0.4</v>
       </c>
-      <c r="C33" s="15">
+      <c r="C33" s="10">
         <v>0.4</v>
       </c>
     </row>
@@ -1467,7 +1487,7 @@
       <c r="A47" t="s">
         <v>49</v>
       </c>
-      <c r="B47" s="15">
+      <c r="B47" s="10">
         <v>0.4</v>
       </c>
       <c r="C47">
@@ -1533,7 +1553,7 @@
       <c r="A53" t="s">
         <v>55</v>
       </c>
-      <c r="B53" s="15">
+      <c r="B53" s="10">
         <v>0.4</v>
       </c>
       <c r="C53">
@@ -1544,7 +1564,7 @@
       <c r="A54" t="s">
         <v>56</v>
       </c>
-      <c r="B54" s="15">
+      <c r="B54" s="10">
         <v>0.4</v>
       </c>
       <c r="C54">
@@ -1588,7 +1608,7 @@
       <c r="A58" t="s">
         <v>60</v>
       </c>
-      <c r="B58" s="15">
+      <c r="B58" s="10">
         <v>0.4</v>
       </c>
       <c r="C58">

</xml_diff>